<commit_message>
Changed Excel and adapted ISI and main
</commit_message>
<xml_diff>
--- a/Design/Burundi final.xlsx
+++ b/Design/Burundi final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabrina\Documents\GitHub\IRP-framework\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A49AF56-B3F3-4F53-8372-7EB5B404326A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5996B9A-7059-4013-8FAD-3AFADF7B7654}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{5975349C-58A3-4B5B-8FE6-1441333428CB}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="220">
   <si>
     <t>Name_ID</t>
   </si>
@@ -762,12 +762,6 @@
   </si>
   <si>
     <t>Lower</t>
-  </si>
-  <si>
-    <t>Inital</t>
-  </si>
-  <si>
-    <t>Capacitiy</t>
   </si>
   <si>
     <t>Fixed Cost</t>
@@ -1227,9 +1221,9 @@
     <tableColumn id="1" xr3:uid="{412BEF91-95C9-4F97-AB74-BDA5528E1CB3}" name="Name" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{05CA1024-D8D3-4457-9A4F-6DE1CBB47D2B}" name="Latitude" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{4C32D59A-9088-4996-B7B2-DF8A1B05203A}" name="Longitude" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{89315792-D525-46B0-A33D-3527CD856DE7}" name="Capacitiy" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{89315792-D525-46B0-A33D-3527CD856DE7}" name="Capacity" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{FAE2B975-1DB4-428D-8894-22256F93BDDE}" name="Lower" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{5412C3A0-F2C5-41BF-AB57-3DA19ECECCCE}" name="Inital" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{5412C3A0-F2C5-41BF-AB57-3DA19ECECCCE}" name="Initial" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{F795114F-5871-4C9B-A276-526B58F4F0AC}" name="Fixed Cost" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1572,16 +1566,16 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>215</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -8844,7 +8838,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8870,10 +8864,10 @@
         <v>215</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -8889,7 +8883,9 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">

</xml_diff>